<commit_message>
Handling Special Chars in Table Names and Column names Done :))
</commit_message>
<xml_diff>
--- a/ExcelUploader/Uploads/Book.xlsx
+++ b/ExcelUploader/Uploads/Book.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -57,6 +57,24 @@
   </si>
   <si>
     <t>Designer</t>
+  </si>
+  <si>
+    <t>dead</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>fav game</t>
+  </si>
+  <si>
+    <t>cod</t>
+  </si>
+  <si>
+    <t>game of throns mob</t>
   </si>
 </sst>
 </file>
@@ -374,15 +392,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" activeCellId="1" sqref="A7:XFD7 A8:XFD8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,8 +410,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -403,8 +427,14 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -414,8 +444,14 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -425,8 +461,11 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -436,8 +475,11 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -447,27 +489,8 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
+      <c r="D6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>